<commit_message>
Added ways to select a product post-query (for special cases)
</commit_message>
<xml_diff>
--- a/externalData/SKU match 4.xlsx
+++ b/externalData/SKU match 4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4150" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4173" uniqueCount="731">
   <si>
     <t>Brand</t>
   </si>
@@ -2389,6 +2389,9 @@
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2396,9 +2399,6 @@
     </xf>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -2449,11 +2449,15 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="6">
+  <tableStyles count="7">
     <tableStyle count="3" pivot="0" name="DataSet-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="DataSet-style 2">
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="Description for Attributes-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
@@ -2549,7 +2553,55 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B5:C14" displayName="Table_2" name="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A217:AN217" displayName="Table_2" name="Table_2" id="2">
+  <tableColumns count="40">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+    <tableColumn name="Column4" id="4"/>
+    <tableColumn name="Column5" id="5"/>
+    <tableColumn name="Column6" id="6"/>
+    <tableColumn name="Column7" id="7"/>
+    <tableColumn name="Column8" id="8"/>
+    <tableColumn name="Column9" id="9"/>
+    <tableColumn name="Column10" id="10"/>
+    <tableColumn name="Column11" id="11"/>
+    <tableColumn name="Column12" id="12"/>
+    <tableColumn name="Column13" id="13"/>
+    <tableColumn name="Column14" id="14"/>
+    <tableColumn name="Column15" id="15"/>
+    <tableColumn name="Column16" id="16"/>
+    <tableColumn name="Column17" id="17"/>
+    <tableColumn name="Column18" id="18"/>
+    <tableColumn name="Column19" id="19"/>
+    <tableColumn name="Column20" id="20"/>
+    <tableColumn name="Column21" id="21"/>
+    <tableColumn name="Column22" id="22"/>
+    <tableColumn name="Column23" id="23"/>
+    <tableColumn name="Column24" id="24"/>
+    <tableColumn name="Column25" id="25"/>
+    <tableColumn name="Column26" id="26"/>
+    <tableColumn name="Column27" id="27"/>
+    <tableColumn name="Column28" id="28"/>
+    <tableColumn name="Column29" id="29"/>
+    <tableColumn name="Column30" id="30"/>
+    <tableColumn name="Column31" id="31"/>
+    <tableColumn name="Column32" id="32"/>
+    <tableColumn name="Column33" id="33"/>
+    <tableColumn name="Column34" id="34"/>
+    <tableColumn name="Column35" id="35"/>
+    <tableColumn name="Column36" id="36"/>
+    <tableColumn name="Column37" id="37"/>
+    <tableColumn name="Column38" id="38"/>
+    <tableColumn name="Column39" id="39"/>
+    <tableColumn name="Column40" id="40"/>
+  </tableColumns>
+  <tableStyleInfo name="DataSet-style 2" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="B5:C14" displayName="Table_3" name="Table_3" id="3">
   <tableColumns count="2">
     <tableColumn name="Attribute" id="1"/>
     <tableColumn name="Description" id="2"/>
@@ -2558,8 +2610,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="E5:F84" displayName="Table_3" name="Table_3" id="3">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="E5:F84" displayName="Table_4" name="Table_4" id="4">
   <tableColumns count="2">
     <tableColumn name="Attribute Vaue" id="1"/>
     <tableColumn name="Description" id="2"/>
@@ -2568,8 +2620,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="H5:J11" displayName="Table_4" name="Table_4" id="4">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="H5:J11" displayName="Table_5" name="Table_5" id="5">
   <tableColumns count="3">
     <tableColumn name="Brand" id="1"/>
     <tableColumn name="Collection Code" id="2"/>
@@ -2579,8 +2631,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="L5:L10" displayName="Table_5" name="Table_5" id="5">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="L5:L10" displayName="Table_6" name="Table_6" id="6">
   <tableColumns count="1">
     <tableColumn name="Type of product" id="1"/>
   </tableColumns>
@@ -2588,8 +2640,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B6:H27" displayName="Table_6" name="Table_6" id="6">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="B6:H27" displayName="Table_7" name="Table_7" id="7">
   <tableColumns count="7">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -21318,7 +21370,94 @@
         <v>584</v>
       </c>
     </row>
-    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1">
+      <c r="A217" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="D217" s="4"/>
+      <c r="E217" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="F217" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G217" s="17" t="s">
+        <v>591</v>
+      </c>
+      <c r="H217" s="17" t="s">
+        <v>592</v>
+      </c>
+      <c r="I217" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="J217" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K217" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L217" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M217" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="N217" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="O217" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="P217" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q217" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="R217" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="S217" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="T217" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="U217" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="V217" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="W217" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="X217" s="4"/>
+      <c r="Y217" s="4"/>
+      <c r="Z217" s="4"/>
+      <c r="AA217" s="4"/>
+      <c r="AB217" s="4"/>
+      <c r="AC217" s="4"/>
+      <c r="AD217" s="4"/>
+      <c r="AE217" s="4"/>
+      <c r="AF217" s="4"/>
+      <c r="AG217" s="4"/>
+      <c r="AH217" s="4"/>
+      <c r="AI217" s="4"/>
+      <c r="AJ217" s="4"/>
+      <c r="AK217" s="4"/>
+      <c r="AL217" s="4"/>
+      <c r="AM217" s="4"/>
+      <c r="AN217" s="16" t="s">
+        <v>584</v>
+      </c>
+    </row>
     <row r="218" ht="15.75" customHeight="1"/>
     <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1"/>
@@ -22116,8 +22255,9 @@
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -22154,7 +22294,7 @@
       <c r="C5" s="4" t="s">
         <v>594</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="18" t="s">
         <v>595</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -22186,7 +22326,7 @@
       <c r="F6" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="19" t="s">
         <v>52</v>
       </c>
       <c r="I6" s="4" t="s">
@@ -22212,7 +22352,7 @@
       <c r="F7" s="4" t="s">
         <v>600</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="19" t="s">
         <v>118</v>
       </c>
       <c r="I7" s="4" t="s">
@@ -22238,7 +22378,7 @@
       <c r="F8" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="19" t="s">
         <v>226</v>
       </c>
       <c r="I8" s="4" t="s">
@@ -22264,7 +22404,7 @@
       <c r="F9" s="4" t="s">
         <v>606</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="19" t="s">
         <v>244</v>
       </c>
       <c r="I9" s="4" t="s">
@@ -22290,7 +22430,7 @@
       <c r="F10" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="19" t="s">
         <v>357</v>
       </c>
       <c r="I10" s="4" t="s">
@@ -22316,7 +22456,7 @@
       <c r="F11" s="4" t="s">
         <v>612</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="19" t="s">
         <v>357</v>
       </c>
       <c r="I11" s="4" t="s">
@@ -24026,10 +24166,10 @@
       <c r="F12" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="20" t="s">
         <v>716</v>
       </c>
-      <c r="H12" s="19"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13">
       <c r="B13" s="10" t="s">
@@ -24048,10 +24188,10 @@
       <c r="F13" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="21" t="s">
         <v>717</v>
       </c>
-      <c r="H13" s="20"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14">
       <c r="B14" s="4" t="s">
@@ -24158,7 +24298,7 @@
       <c r="F18" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="20" t="s">
         <v>722</v>
       </c>
       <c r="H18" s="4"/>
@@ -24180,7 +24320,7 @@
       <c r="F19" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="21" t="s">
         <v>723</v>
       </c>
       <c r="H19" s="4"/>
@@ -24192,7 +24332,7 @@
       <c r="C20" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="22" t="s">
         <v>345</v>
       </c>
       <c r="E20" s="7" t="s">
@@ -24201,7 +24341,7 @@
       <c r="F20" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="20" t="s">
         <v>724</v>
       </c>
       <c r="H20" s="4"/>
@@ -24213,7 +24353,7 @@
       <c r="C21" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="22" t="s">
         <v>345</v>
       </c>
       <c r="E21" s="10" t="s">
@@ -24222,7 +24362,7 @@
       <c r="F21" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="21" t="s">
         <v>725</v>
       </c>
       <c r="H21" s="4"/>
@@ -24326,10 +24466,10 @@
         <f t="array" ref="D26">XLOOKUP('Picture Set Up'!$C26,DataSet!$B$7:$B$216,DataSet!$C$7:$C$216,"")</f>
         <v>Glasklar</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="17" t="s">
         <v>341</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F26" s="17" t="s">
         <v>520</v>
       </c>
       <c r="G26" s="23" t="s">

</xml_diff>